<commit_message>
Add difot score template export
</commit_message>
<xml_diff>
--- a/src/private/templates/difot_score.xlsx
+++ b/src/private/templates/difot_score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,21 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>date</t>
+    <t>SAP No</t>
   </si>
   <si>
-    <t>amount</t>
+    <t>Supplier name</t>
   </si>
   <si>
-    <t>name</t>
+    <t>DIFOT score</t>
   </si>
   <si>
-    <t>batamar</t>
-  </si>
-  <si>
-    <t>supplierName</t>
+    <t>Month/Year</t>
   </si>
 </sst>
 </file>
@@ -74,9 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,11 +350,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -367,37 +361,18 @@
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>43893</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43446</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced sap number words in excel files
</commit_message>
<xml_diff>
--- a/src/private/templates/difot_score.xlsx
+++ b/src/private/templates/difot_score.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>SAP No</t>
-  </si>
-  <si>
     <t>Supplier name</t>
   </si>
   <si>
@@ -36,6 +33,9 @@
   </si>
   <si>
     <t>Month/Year</t>
+  </si>
+  <si>
+    <t>Vendor number</t>
   </si>
 </sst>
 </file>
@@ -363,16 +363,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>